<commit_message>
still on classification 2
Added images;
</commit_message>
<xml_diff>
--- a/R/CH83-ClassificationTask/File1.xlsx
+++ b/R/CH83-ClassificationTask/File1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafrocBook/R/CH83-ClassificationTask/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8940CF23-2D14-6B4A-99A9-B08C0A50A2CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D3AF28-B618-3F4E-9986-A8AFC5F502F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18120" yWindow="460" windowWidth="10000" windowHeight="8000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1806,9 +1806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1858,7 +1856,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
update to FP png sheets in classification chapter
* ClassRx to ClassDx
* Other minor edits
</commit_message>
<xml_diff>
--- a/R/CH83-ClassificationTask/File1.xlsx
+++ b/R/CH83-ClassificationTask/File1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafrocBook/R/CH83-ClassificationTask/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D3AF28-B618-3F4E-9986-A8AFC5F502F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78197D1D-3340-CD43-BFFA-9E26D11A1AFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18120" yWindow="460" windowWidth="10000" windowHeight="8000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,9 +109,6 @@
     <t>ClassTrue</t>
   </si>
   <si>
-    <t>ClassRx</t>
-  </si>
-  <si>
     <t>CL-IC</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>ClassDx</t>
   </si>
 </sst>
 </file>
@@ -1670,7 +1670,7 @@
         <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1690,10 +1690,10 @@
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1713,10 +1713,10 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1736,10 +1736,10 @@
         <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1759,10 +1759,10 @@
         <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1782,10 +1782,10 @@
         <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1806,7 +1806,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1836,7 +1838,7 @@
         <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1853,16 +1855,16 @@
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1879,13 +1881,13 @@
         <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1899,16 +1901,16 @@
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1925,13 +1927,13 @@
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1948,13 +1950,13 @@
         <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1971,13 +1973,13 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1994,13 +1996,13 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2052,10 +2054,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2075,10 +2077,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2098,10 +2100,10 @@
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2122,7 +2124,7 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2143,7 +2145,7 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -2164,7 +2166,7 @@
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2185,7 +2187,7 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2206,7 +2208,7 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>